<commit_message>
Introduce validator for OASI numbers
</commit_message>
<xml_diff>
--- a/demo/src/data/NodeHelvetiaExcel-Input.xlsx
+++ b/demo/src/data/NodeHelvetiaExcel-Input.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10513"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF8C0A1-3C0B-3C46-BC75-C82CFBF09E2E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22035" windowHeight="14580"/>
+    <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Austritte" sheetId="1" r:id="rId1"/>
@@ -15,12 +16,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -30,7 +31,7 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -44,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -54,7 +55,7 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -73,12 +74,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -88,7 +89,7 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -102,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -112,7 +113,7 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -126,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -136,7 +137,7 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>Autor:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -155,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="52">
   <si>
     <t>AHV-Nummer</t>
   </si>
@@ -236,30 +237,6 @@
     <t>Swisscanto Sammelstiftungen</t>
   </si>
   <si>
-    <t>7562449375258</t>
-  </si>
-  <si>
-    <t>7566327722938</t>
-  </si>
-  <si>
-    <t>7564432926738</t>
-  </si>
-  <si>
-    <t>7569088848466</t>
-  </si>
-  <si>
-    <t>7567912791961</t>
-  </si>
-  <si>
-    <t>7566763705098</t>
-  </si>
-  <si>
-    <t>7567808877566</t>
-  </si>
-  <si>
-    <t>7568824253347</t>
-  </si>
-  <si>
     <t>Ref HV 1</t>
   </si>
   <si>
@@ -312,13 +289,37 @@
   </si>
   <si>
     <t>7564364963317</t>
+  </si>
+  <si>
+    <t>7567912791967</t>
+  </si>
+  <si>
+    <t>7566763705093</t>
+  </si>
+  <si>
+    <t>7567808877560</t>
+  </si>
+  <si>
+    <t>7568824253345</t>
+  </si>
+  <si>
+    <t>7562449375253</t>
+  </si>
+  <si>
+    <t>7566327722931</t>
+  </si>
+  <si>
+    <t>7564432926732</t>
+  </si>
+  <si>
+    <t>7569088848469</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,7 +410,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -434,6 +435,10 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -442,9 +447,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Überschrift 3" xfId="2" builtinId="18"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -460,7 +465,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -535,6 +540,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -570,6 +592,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -745,29 +784,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="21.59765625" customWidth="1"/>
-    <col min="3" max="3" width="17.3984375" customWidth="1"/>
+    <col min="1" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="4" width="84" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4" ht="20" thickBot="1">
+      <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -781,9 +820,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4">
       <c r="A3" s="11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4">
         <v>43252</v>
@@ -792,12 +831,12 @@
         <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B4" s="4">
         <v>43221</v>
@@ -806,12 +845,12 @@
         <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>50</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="B5" s="4">
         <v>43252</v>
@@ -820,12 +859,12 @@
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>51</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="B6" s="4">
         <v>43221</v>
@@ -834,12 +873,12 @@
         <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B7" s="4">
         <v>43252</v>
@@ -848,12 +887,12 @@
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="B8" s="4">
         <v>43221</v>
@@ -862,12 +901,12 @@
         <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="12" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>32</v>
       </c>
       <c r="B9" s="4">
         <v>43252</v>
@@ -876,12 +915,12 @@
         <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="B10" s="4">
         <v>43221</v>
@@ -890,412 +929,412 @@
         <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4">
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4">
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:2">
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:2">
       <c r="B18" s="5"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:2">
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:2">
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:2">
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:2">
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:2">
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:2">
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:2">
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:2">
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:2">
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:2">
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:2">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:2">
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:2">
       <c r="B31" s="5"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:2">
       <c r="B32" s="5"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2">
       <c r="B33" s="5"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:2">
       <c r="B34" s="5"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:2">
       <c r="B35" s="5"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:2">
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:2">
       <c r="B37" s="5"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:2">
       <c r="B38" s="5"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:2">
       <c r="B39" s="5"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:2">
       <c r="B40" s="5"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:2">
       <c r="B41" s="5"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:2">
       <c r="B42" s="5"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:2">
       <c r="B43" s="5"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:2">
       <c r="B44" s="5"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:2">
       <c r="B45" s="5"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:2">
       <c r="B46" s="5"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:2">
       <c r="B47" s="5"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:2">
       <c r="B48" s="5"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:2">
       <c r="B49" s="5"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:2">
       <c r="B50" s="5"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:2">
       <c r="B51" s="5"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:2">
       <c r="B52" s="5"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:2">
       <c r="B53" s="5"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:2">
       <c r="B54" s="5"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:2">
       <c r="B55" s="5"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:2">
       <c r="B56" s="5"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:2">
       <c r="B57" s="5"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:2">
       <c r="B58" s="5"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:2">
       <c r="B59" s="5"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:2">
       <c r="B60" s="5"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:2">
       <c r="B61" s="5"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:2">
       <c r="B62" s="5"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:2">
       <c r="B63" s="5"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:2">
       <c r="B64" s="5"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:2">
       <c r="B65" s="5"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:2">
       <c r="B66" s="5"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:2">
       <c r="B67" s="5"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:2">
       <c r="B68" s="5"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:2">
       <c r="B69" s="5"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:2">
       <c r="B70" s="5"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:2">
       <c r="B71" s="5"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:2">
       <c r="B72" s="5"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:2">
       <c r="B73" s="5"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:2">
       <c r="B74" s="5"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:2">
       <c r="B75" s="5"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:2">
       <c r="B76" s="5"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:2">
       <c r="B77" s="5"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:2">
       <c r="B78" s="5"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:2">
       <c r="B79" s="5"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:2">
       <c r="B80" s="5"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:2">
       <c r="B81" s="5"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:2">
       <c r="B82" s="5"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:2">
       <c r="B83" s="5"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:2">
       <c r="B84" s="5"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:2">
       <c r="B85" s="5"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:2">
       <c r="B86" s="5"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:2">
       <c r="B87" s="5"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:2">
       <c r="B88" s="5"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:2">
       <c r="B89" s="5"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:2">
       <c r="B90" s="5"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="2:2">
       <c r="B91" s="5"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="2:2">
       <c r="B92" s="5"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="2:2">
       <c r="B93" s="5"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="2:2">
       <c r="B94" s="5"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="2:2">
       <c r="B95" s="5"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="2:2">
       <c r="B96" s="5"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="2:2">
       <c r="B97" s="5"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="2:2">
       <c r="B98" s="5"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="99" spans="2:2">
       <c r="B99" s="5"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="2:2">
       <c r="B100" s="5"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="2:2">
       <c r="B101" s="5"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="2:2">
       <c r="B102" s="5"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="103" spans="2:2">
       <c r="B103" s="5"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="104" spans="2:2">
       <c r="B104" s="5"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="2:2">
       <c r="B105" s="5"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="106" spans="2:2">
       <c r="B106" s="5"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="107" spans="2:2">
       <c r="B107" s="5"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="108" spans="2:2">
       <c r="B108" s="5"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="2:2">
       <c r="B109" s="5"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="110" spans="2:2">
       <c r="B110" s="5"/>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="111" spans="2:2">
       <c r="B111" s="5"/>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="112" spans="2:2">
       <c r="B112" s="5"/>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="113" spans="2:2">
       <c r="B113" s="5"/>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="114" spans="2:2">
       <c r="B114" s="5"/>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="115" spans="2:2">
       <c r="B115" s="5"/>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="116" spans="2:2">
       <c r="B116" s="5"/>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="117" spans="2:2">
       <c r="B117" s="5"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="118" spans="2:2">
       <c r="B118" s="5"/>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="119" spans="2:2">
       <c r="B119" s="5"/>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="120" spans="2:2">
       <c r="B120" s="5"/>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="121" spans="2:2">
       <c r="B121" s="5"/>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="122" spans="2:2">
       <c r="B122" s="5"/>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="123" spans="2:2">
       <c r="B123" s="5"/>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="124" spans="2:2">
       <c r="B124" s="5"/>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="125" spans="2:2">
       <c r="B125" s="5"/>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="126" spans="2:2">
       <c r="B126" s="5"/>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="127" spans="2:2">
       <c r="B127" s="5"/>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="128" spans="2:2">
       <c r="B128" s="5"/>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="129" spans="2:2">
       <c r="B129" s="5"/>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="130" spans="2:2">
       <c r="B130" s="5"/>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="131" spans="2:2">
       <c r="B131" s="5"/>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="132" spans="2:2">
       <c r="B132" s="5"/>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="133" spans="2:2">
       <c r="B133" s="5"/>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="134" spans="2:2">
       <c r="B134" s="5"/>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="135" spans="2:2">
       <c r="B135" s="5"/>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="136" spans="2:2">
       <c r="B136" s="5"/>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="137" spans="2:2">
       <c r="B137" s="5"/>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="138" spans="2:2">
       <c r="B138" s="5"/>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="139" spans="2:2">
       <c r="B139" s="5"/>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="140" spans="2:2">
       <c r="B140" s="5"/>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="141" spans="2:2">
       <c r="B141" s="5"/>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="142" spans="2:2">
       <c r="B142" s="5"/>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="143" spans="2:2">
       <c r="B143" s="5"/>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="144" spans="2:2">
       <c r="B144" s="5"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="145" spans="2:2">
       <c r="B145" s="5"/>
     </row>
   </sheetData>
@@ -1309,39 +1348,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="21.59765625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="17.3984375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="67.1328125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="36.53125" style="6" customWidth="1"/>
-    <col min="7" max="9" width="21.59765625" style="6" customWidth="1"/>
+    <col min="1" max="2" width="21.6640625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="17.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="67.1640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="36.5" style="6" customWidth="1"/>
+    <col min="7" max="9" width="21.6640625" style="6" customWidth="1"/>
     <col min="10" max="10" width="24" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="9.1328125" style="6"/>
+    <col min="11" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:10" ht="20" thickBot="1">
+      <c r="A1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-    </row>
-    <row r="2" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+    </row>
+    <row r="2" spans="1:10" ht="17" thickTop="1" thickBot="1">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1373,7 +1412,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" ht="57" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -1384,7 +1423,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>20</v>
@@ -1401,9 +1440,11 @@
       <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="J3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -1414,7 +1455,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>20</v>
@@ -1431,10 +1472,12 @@
       <c r="I4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="6" t="s">
+      <c r="J4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45">
+      <c r="A5" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="10">
@@ -1444,7 +1487,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>25</v>
@@ -1465,8 +1508,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:10" ht="45">
+      <c r="A6" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="10">
@@ -1476,7 +1519,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>25</v>
@@ -1493,9 +1536,12 @@
       <c r="I6" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="6" t="s">
+      <c r="J6" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45">
+      <c r="A7" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="10">
@@ -1505,7 +1551,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>20</v>
@@ -1522,9 +1568,12 @@
       <c r="I7" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A8" s="6" t="s">
+      <c r="J7" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="45">
+      <c r="A8" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="10">
@@ -1534,7 +1583,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>20</v>
@@ -1551,10 +1600,13 @@
       <c r="I8" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" s="6" t="s">
-        <v>26</v>
+      <c r="J8" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="B9" s="10">
         <v>43344</v>
@@ -1563,7 +1615,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>25</v>
@@ -1584,9 +1636,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="6" t="s">
-        <v>27</v>
+    <row r="10" spans="1:10">
+      <c r="A10" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="B10" s="10">
         <v>43339</v>
@@ -1595,7 +1647,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>25</v>
@@ -1612,10 +1664,13 @@
       <c r="I10" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" s="6" t="s">
-        <v>28</v>
+      <c r="J10" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="B11" s="10">
         <v>43346</v>
@@ -1624,7 +1679,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>20</v>
@@ -1641,10 +1696,13 @@
       <c r="I11" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" s="6" t="s">
-        <v>29</v>
+      <c r="J11" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="B12" s="10">
         <v>43325</v>
@@ -1653,7 +1711,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>20</v>
@@ -1670,263 +1728,266 @@
       <c r="I12" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J12" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10">
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10">
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:2">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:2">
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:2">
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:2">
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:2">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:2">
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:2">
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:2">
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:2">
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:2">
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:2">
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:2">
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:2">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:2">
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:2">
       <c r="B31" s="10"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:2">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2">
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:2">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:2">
       <c r="B35" s="10"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:2">
       <c r="B36" s="10"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:2">
       <c r="B37" s="10"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:2">
       <c r="B38" s="10"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:2">
       <c r="B39" s="10"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:2">
       <c r="B40" s="10"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:2">
       <c r="B41" s="10"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:2">
       <c r="B42" s="10"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:2">
       <c r="B43" s="10"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:2">
       <c r="B44" s="10"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:2">
       <c r="B45" s="10"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:2">
       <c r="B46" s="10"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:2">
       <c r="B47" s="10"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:2">
       <c r="B48" s="10"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:2">
       <c r="B49" s="10"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:2">
       <c r="B50" s="10"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:2">
       <c r="B51" s="10"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:2">
       <c r="B52" s="10"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:2">
       <c r="B53" s="10"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:2">
       <c r="B54" s="10"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:2">
       <c r="B55" s="10"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:2">
       <c r="B56" s="10"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:2">
       <c r="B57" s="10"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:2">
       <c r="B58" s="10"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:2">
       <c r="B59" s="10"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:2">
       <c r="B60" s="10"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:2">
       <c r="B61" s="10"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:2">
       <c r="B62" s="10"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:2">
       <c r="B63" s="10"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:2">
       <c r="B64" s="10"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:2">
       <c r="B65" s="10"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:2">
       <c r="B66" s="10"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:2">
       <c r="B67" s="10"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:2">
       <c r="B68" s="10"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:2">
       <c r="B69" s="10"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:2">
       <c r="B70" s="10"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:2">
       <c r="B71" s="10"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:2">
       <c r="B72" s="10"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:2">
       <c r="B73" s="10"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:2">
       <c r="B74" s="10"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:2">
       <c r="B75" s="10"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:2">
       <c r="B76" s="10"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:2">
       <c r="B77" s="10"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:2">
       <c r="B78" s="10"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:2">
       <c r="B79" s="10"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:2">
       <c r="B80" s="10"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:2">
       <c r="B81" s="10"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:2">
       <c r="B82" s="10"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:2">
       <c r="B83" s="10"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:2">
       <c r="B84" s="10"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:2">
       <c r="B85" s="10"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:2">
       <c r="B86" s="10"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:2">
       <c r="B87" s="10"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:2">
       <c r="B88" s="10"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:2">
       <c r="B89" s="10"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:2">
       <c r="B90" s="10"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="2:2">
       <c r="B91" s="10"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="2:2">
       <c r="B92" s="10"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="2:2">
       <c r="B93" s="10"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="2:2">
       <c r="B94" s="10"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="2:2">
       <c r="B95" s="10"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="2:2">
       <c r="B96" s="10"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="2:2">
       <c r="B97" s="10"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="2:2">
       <c r="B98" s="10"/>
     </row>
   </sheetData>

</xml_diff>